<commit_message>
Great Depression and Financial Crisis Notebook, Companion to Crisis and Credit Allocation
</commit_message>
<xml_diff>
--- a/Advanced Macroeconomics/Course Notes/fedData.xlsx
+++ b/Advanced Macroeconomics/Course Notes/fedData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLCat\OneDrive\Documents\For NDSU\Projects\My Projects\Hayek on Gold\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLCat\GithubRepositories\Macroeconomics-Growth-and-Monetary-Equilibrium\Advanced Macroeconomics\Course Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C958B6-3B19-4BAA-8B77-9847749B0FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05E0B3-AC4F-4F08-9E05-7EF74B790CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="2262" windowWidth="17280" windowHeight="9444" xr2:uid="{FCF80F92-4F73-4BE5-8F52-4F3690825380}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCF80F92-4F73-4BE5-8F52-4F3690825380}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>High Powered Money (mil) (Friedman Schwartz)</t>
-  </si>
   <si>
     <t>High Powered Money Less Gold</t>
   </si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>Gold</t>
+  </si>
+  <si>
+    <t>High Powered Money (mil)</t>
   </si>
 </sst>
 </file>
@@ -427,53 +427,53 @@
   <dimension ref="A1:L379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="10.578125" customWidth="1"/>
+    <col min="2" max="4" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>6576</v>
       </c>
@@ -487,7 +487,7 @@
         <v>2640</v>
       </c>
       <c r="E2" s="1">
-        <f>B2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">B2/D2</f>
         <v>2.0882575757575759</v>
       </c>
       <c r="F2">
@@ -512,7 +512,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>6607</v>
       </c>
@@ -526,7 +526,7 @@
         <v>2833</v>
       </c>
       <c r="E3" s="1">
-        <f>B3/D3</f>
+        <f t="shared" si="0"/>
         <v>2.0148252735615957</v>
       </c>
       <c r="F3">
@@ -551,7 +551,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>6635</v>
       </c>
@@ -565,7 +565,7 @@
         <v>2935</v>
       </c>
       <c r="E4" s="1">
-        <f>B4/D4</f>
+        <f t="shared" si="0"/>
         <v>1.9805792163543441</v>
       </c>
       <c r="F4">
@@ -590,7 +590,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>6666</v>
       </c>
@@ -604,7 +604,7 @@
         <v>3013</v>
       </c>
       <c r="E5" s="1">
-        <f>B5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.9555260537670096</v>
       </c>
       <c r="F5">
@@ -629,7 +629,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>6696</v>
       </c>
@@ -643,7 +643,7 @@
         <v>2970</v>
       </c>
       <c r="E6" s="1">
-        <f>B6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.9713804713804715</v>
       </c>
       <c r="F6">
@@ -668,7 +668,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6727</v>
       </c>
@@ -682,7 +682,7 @@
         <v>3016</v>
       </c>
       <c r="E7" s="1">
-        <f>B7/D7</f>
+        <f t="shared" si="0"/>
         <v>1.953580901856764</v>
       </c>
       <c r="F7">
@@ -707,7 +707,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6757</v>
       </c>
@@ -721,7 +721,7 @@
         <v>3107</v>
       </c>
       <c r="E8" s="1">
-        <f>B8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.9253299002252977</v>
       </c>
       <c r="F8">
@@ -746,7 +746,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6788</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3344</v>
       </c>
       <c r="E9" s="1">
-        <f>B9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.8594497607655502</v>
       </c>
       <c r="F9">
@@ -785,7 +785,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>6819</v>
       </c>
@@ -799,7 +799,7 @@
         <v>3552</v>
       </c>
       <c r="E10" s="1">
-        <f>B10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.8068693693693694</v>
       </c>
       <c r="F10">
@@ -824,7 +824,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>6849</v>
       </c>
@@ -838,7 +838,7 @@
         <v>3802</v>
       </c>
       <c r="E11" s="1">
-        <f>B11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.7546028406102052</v>
       </c>
       <c r="F11">
@@ -863,7 +863,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>6880</v>
       </c>
@@ -877,7 +877,7 @@
         <v>3571</v>
       </c>
       <c r="E12" s="1">
-        <f>B12/D12</f>
+        <f t="shared" si="0"/>
         <v>1.8042565107812938</v>
       </c>
       <c r="F12">
@@ -902,7 +902,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>6910</v>
       </c>
@@ -916,7 +916,7 @@
         <v>3656</v>
       </c>
       <c r="E13" s="1">
-        <f>B13/D13</f>
+        <f t="shared" si="0"/>
         <v>1.7858315098468271</v>
       </c>
       <c r="F13">
@@ -941,7 +941,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>6941</v>
       </c>
@@ -955,7 +955,7 @@
         <v>3586</v>
       </c>
       <c r="E14" s="1">
-        <f>B14/D14</f>
+        <f t="shared" si="0"/>
         <v>1.8017289459007251</v>
       </c>
       <c r="F14">
@@ -980,7 +980,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>6972</v>
       </c>
@@ -994,7 +994,7 @@
         <v>3549</v>
       </c>
       <c r="E15" s="1">
-        <f>B15/D15</f>
+        <f t="shared" si="0"/>
         <v>1.8109326570865032</v>
       </c>
       <c r="F15">
@@ -1019,7 +1019,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>7000</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>3584</v>
       </c>
       <c r="E16" s="1">
-        <f>B16/D16</f>
+        <f t="shared" si="0"/>
         <v>1.8030133928571428</v>
       </c>
       <c r="F16">
@@ -1058,7 +1058,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>7031</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>3679</v>
       </c>
       <c r="E17" s="1">
-        <f>B17/D17</f>
+        <f t="shared" si="0"/>
         <v>1.7855395487904322</v>
       </c>
       <c r="F17">
@@ -1097,7 +1097,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7061</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>3673</v>
       </c>
       <c r="E18" s="1">
-        <f>B18/D18</f>
+        <f t="shared" si="0"/>
         <v>1.7868227606860876</v>
       </c>
       <c r="F18">
@@ -1136,7 +1136,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>7092</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>3691</v>
       </c>
       <c r="E19" s="1">
-        <f>B19/D19</f>
+        <f t="shared" si="0"/>
         <v>1.7656461663505825</v>
       </c>
       <c r="F19">
@@ -1175,7 +1175,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>7122</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>3816</v>
       </c>
       <c r="E20" s="1">
-        <f>B20/D20</f>
+        <f t="shared" si="0"/>
         <v>1.7277253668763102</v>
       </c>
       <c r="F20">
@@ -1214,7 +1214,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>7153</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>3797</v>
       </c>
       <c r="E21" s="1">
-        <f>B21/D21</f>
+        <f t="shared" si="0"/>
         <v>1.7474321833026074</v>
       </c>
       <c r="F21">
@@ -1253,7 +1253,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>7184</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>3811</v>
       </c>
       <c r="E22" s="1">
-        <f>B22/D22</f>
+        <f t="shared" si="0"/>
         <v>1.7504591970611387</v>
       </c>
       <c r="F22">
@@ -1292,7 +1292,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>7214</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>3977</v>
       </c>
       <c r="E23" s="1">
-        <f>B23/D23</f>
+        <f t="shared" si="0"/>
         <v>1.7080714106110133</v>
       </c>
       <c r="F23">
@@ -1331,7 +1331,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>7245</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>4117</v>
       </c>
       <c r="E24" s="1">
-        <f>B24/D24</f>
+        <f t="shared" si="0"/>
         <v>1.6696623755161526</v>
       </c>
       <c r="F24">
@@ -1370,7 +1370,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7275</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>4167</v>
       </c>
       <c r="E25" s="1">
-        <f>B25/D25</f>
+        <f t="shared" si="0"/>
         <v>1.6496280297576194</v>
       </c>
       <c r="F25">
@@ -1409,7 +1409,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>7306</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>4266</v>
       </c>
       <c r="E26" s="1">
-        <f>B26/D26</f>
+        <f t="shared" si="0"/>
         <v>1.6195499296765119</v>
       </c>
       <c r="F26">
@@ -1448,7 +1448,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7337</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>4459</v>
       </c>
       <c r="E27" s="1">
-        <f>B27/D27</f>
+        <f t="shared" si="0"/>
         <v>1.5830903790087463</v>
       </c>
       <c r="F27">
@@ -1487,7 +1487,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7366</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>4571</v>
       </c>
       <c r="E28" s="1">
-        <f>B28/D28</f>
+        <f t="shared" si="0"/>
         <v>1.5607088164515424</v>
       </c>
       <c r="F28">
@@ -1526,7 +1526,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7397</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>4648</v>
       </c>
       <c r="E29" s="1">
-        <f>B29/D29</f>
+        <f t="shared" si="0"/>
         <v>1.5494836488812394</v>
       </c>
       <c r="F29">
@@ -1565,7 +1565,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>7427</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>4626</v>
       </c>
       <c r="E30" s="1">
-        <f>B30/D30</f>
+        <f t="shared" si="0"/>
         <v>1.5553393860786857</v>
       </c>
       <c r="F30">
@@ -1604,7 +1604,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>7458</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>4636</v>
       </c>
       <c r="E31" s="1">
-        <f>B31/D31</f>
+        <f t="shared" si="0"/>
         <v>1.5560828300258844</v>
       </c>
       <c r="F31">
@@ -1643,7 +1643,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>7488</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>4678</v>
       </c>
       <c r="E32" s="1">
-        <f>B32/D32</f>
+        <f t="shared" si="0"/>
         <v>1.5504489097905088</v>
       </c>
       <c r="F32">
@@ -1682,7 +1682,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>7519</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>4740</v>
       </c>
       <c r="E33" s="1">
-        <f>B33/D33</f>
+        <f t="shared" si="0"/>
         <v>1.540928270042194</v>
       </c>
       <c r="F33">
@@ -1721,7 +1721,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>7550</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>4709</v>
       </c>
       <c r="E34" s="1">
-        <f>B34/D34</f>
+        <f t="shared" ref="E34:E65" si="1">B34/D34</f>
         <v>1.5491611807177745</v>
       </c>
       <c r="F34">
@@ -1760,7 +1760,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>7580</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>4749</v>
       </c>
       <c r="E35" s="1">
-        <f>B35/D35</f>
+        <f t="shared" si="1"/>
         <v>1.5434828384923143</v>
       </c>
       <c r="F35">
@@ -1799,7 +1799,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>7611</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>4571</v>
       </c>
       <c r="E36" s="1">
-        <f>B36/D36</f>
+        <f t="shared" si="1"/>
         <v>1.5709910304091008</v>
       </c>
       <c r="F36">
@@ -1838,7 +1838,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>7641</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>4534</v>
       </c>
       <c r="E37" s="1">
-        <f>B37/D37</f>
+        <f t="shared" si="1"/>
         <v>1.582046757829731</v>
       </c>
       <c r="F37">
@@ -1877,7 +1877,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>7672</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>4276</v>
       </c>
       <c r="E38" s="1">
-        <f>B38/D38</f>
+        <f t="shared" si="1"/>
         <v>1.6265201122544435</v>
       </c>
       <c r="F38">
@@ -1916,7 +1916,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>7703</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>4175</v>
       </c>
       <c r="E39" s="1">
-        <f>B39/D39</f>
+        <f t="shared" si="1"/>
         <v>1.6498203592814371</v>
       </c>
       <c r="F39">
@@ -1955,7 +1955,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>7731</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>3954</v>
       </c>
       <c r="E40" s="1">
-        <f>B40/D40</f>
+        <f t="shared" si="1"/>
         <v>1.7078907435508346</v>
       </c>
       <c r="F40">
@@ -1994,7 +1994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>7762</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>3848</v>
       </c>
       <c r="E41" s="1">
-        <f>B41/D41</f>
+        <f t="shared" si="1"/>
         <v>1.7476611226611227</v>
       </c>
       <c r="F41">
@@ -2033,7 +2033,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>7792</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>3694</v>
       </c>
       <c r="E42" s="1">
-        <f>B42/D42</f>
+        <f t="shared" si="1"/>
         <v>1.7969680563075257</v>
       </c>
       <c r="F42">
@@ -2072,7 +2072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>7823</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>3561</v>
       </c>
       <c r="E43" s="1">
-        <f>B43/D43</f>
+        <f t="shared" si="1"/>
         <v>1.8390901432181972</v>
       </c>
       <c r="F43">
@@ -2111,7 +2111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>7853</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>3410</v>
       </c>
       <c r="E44" s="1">
-        <f>B44/D44</f>
+        <f t="shared" si="1"/>
         <v>1.8973607038123168</v>
       </c>
       <c r="F44">
@@ -2150,7 +2150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>7884</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>3224</v>
       </c>
       <c r="E45" s="1">
-        <f>B45/D45</f>
+        <f t="shared" si="1"/>
         <v>1.977667493796526</v>
       </c>
       <c r="F45">
@@ -2189,7 +2189,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>7915</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>3154</v>
       </c>
       <c r="E46" s="1">
-        <f>B46/D46</f>
+        <f t="shared" si="1"/>
         <v>2.0247305009511729</v>
       </c>
       <c r="F46">
@@ -2228,7 +2228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>7945</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>2977</v>
       </c>
       <c r="E47" s="1">
-        <f>B47/D47</f>
+        <f t="shared" si="1"/>
         <v>2.1034598589183742</v>
       </c>
       <c r="F47">
@@ -2267,7 +2267,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>7976</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>2875</v>
       </c>
       <c r="E48" s="1">
-        <f>B48/D48</f>
+        <f t="shared" si="1"/>
         <v>2.1617391304347828</v>
       </c>
       <c r="F48">
@@ -2306,7 +2306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>8006</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>2873</v>
       </c>
       <c r="E49" s="1">
-        <f>B49/D49</f>
+        <f t="shared" si="1"/>
         <v>2.1740341106856942</v>
       </c>
       <c r="F49">
@@ -2345,7 +2345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>8037</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>2687</v>
       </c>
       <c r="E50" s="1">
-        <f>B50/D50</f>
+        <f t="shared" si="1"/>
         <v>2.2646073688128023</v>
       </c>
       <c r="F50">
@@ -2384,7 +2384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>8068</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>2706</v>
       </c>
       <c r="E51" s="1">
-        <f>B51/D51</f>
+        <f t="shared" si="1"/>
         <v>2.2697708795269769</v>
       </c>
       <c r="F51">
@@ -2423,7 +2423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>8096</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>2763</v>
       </c>
       <c r="E52" s="1">
-        <f>B52/D52</f>
+        <f t="shared" si="1"/>
         <v>2.2533478103510678</v>
       </c>
       <c r="F52">
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>8127</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>2744</v>
       </c>
       <c r="E53" s="1">
-        <f>B53/D53</f>
+        <f t="shared" si="1"/>
         <v>2.2671282798833818</v>
       </c>
       <c r="F53">
@@ -2501,7 +2501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>8157</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>2778</v>
       </c>
       <c r="E54" s="1">
-        <f>B54/D54</f>
+        <f t="shared" si="1"/>
         <v>2.2541396688264941</v>
       </c>
       <c r="F54">
@@ -2540,7 +2540,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>8188</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>2823</v>
       </c>
       <c r="E55" s="1">
-        <f>B55/D55</f>
+        <f t="shared" si="1"/>
         <v>2.2391073326248669</v>
       </c>
       <c r="F55">
@@ -2579,7 +2579,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>8218</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>2711</v>
       </c>
       <c r="E56" s="1">
-        <f>B56/D56</f>
+        <f t="shared" si="1"/>
         <v>2.3065289561047586</v>
       </c>
       <c r="F56">
@@ -2618,7 +2618,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>8249</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>2727</v>
       </c>
       <c r="E57" s="1">
-        <f>B57/D57</f>
+        <f t="shared" si="1"/>
         <v>2.3083975064173083</v>
       </c>
       <c r="F57">
@@ -2657,7 +2657,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>8280</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>2772</v>
       </c>
       <c r="E58" s="1">
-        <f>B58/D58</f>
+        <f t="shared" si="1"/>
         <v>2.2936507936507935</v>
       </c>
       <c r="F58">
@@ -2696,7 +2696,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>8310</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>2738</v>
       </c>
       <c r="E59" s="1">
-        <f>B59/D59</f>
+        <f t="shared" si="1"/>
         <v>2.3151935719503287</v>
       </c>
       <c r="F59">
@@ -2735,7 +2735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>8341</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>2804</v>
       </c>
       <c r="E60" s="1">
-        <f>B60/D60</f>
+        <f t="shared" si="1"/>
         <v>2.2906562054208273</v>
       </c>
       <c r="F60">
@@ -2774,7 +2774,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>8371</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>2834</v>
       </c>
       <c r="E61" s="1">
-        <f>B61/D61</f>
+        <f t="shared" si="1"/>
         <v>2.285109386026817</v>
       </c>
       <c r="F61">
@@ -2813,7 +2813,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>8402</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>2866</v>
       </c>
       <c r="E62" s="1">
-        <f>B62/D62</f>
+        <f t="shared" si="1"/>
         <v>2.2791346824842988</v>
       </c>
       <c r="F62">
@@ -2852,7 +2852,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>8433</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>2869</v>
       </c>
       <c r="E63" s="1">
-        <f>B63/D63</f>
+        <f t="shared" si="1"/>
         <v>2.2812826768909029</v>
       </c>
       <c r="F63">
@@ -2891,7 +2891,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>8461</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>2941</v>
       </c>
       <c r="E64" s="1">
-        <f>B64/D64</f>
+        <f t="shared" si="1"/>
         <v>2.2522951377082623</v>
       </c>
       <c r="F64">
@@ -2930,7 +2930,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>8492</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>2912</v>
       </c>
       <c r="E65" s="1">
-        <f>B65/D65</f>
+        <f t="shared" si="1"/>
         <v>2.2688873626373627</v>
       </c>
       <c r="F65">
@@ -2969,7 +2969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>8522</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>2939</v>
       </c>
       <c r="E66" s="1">
-        <f>B66/D66</f>
+        <f t="shared" ref="E66:E97" si="2">B66/D66</f>
         <v>2.2728819326301464</v>
       </c>
       <c r="F66">
@@ -3008,7 +3008,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>8553</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>2919</v>
       </c>
       <c r="E67" s="1">
-        <f>B67/D67</f>
+        <f t="shared" si="2"/>
         <v>2.2891401164782459</v>
       </c>
       <c r="F67">
@@ -3047,7 +3047,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>8583</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>2878</v>
       </c>
       <c r="E68" s="1">
-        <f>B68/D68</f>
+        <f t="shared" si="2"/>
         <v>2.3175816539263376</v>
       </c>
       <c r="F68">
@@ -3086,7 +3086,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>8614</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>2910</v>
       </c>
       <c r="E69" s="1">
-        <f>B69/D69</f>
+        <f t="shared" si="2"/>
         <v>2.314089347079038</v>
       </c>
       <c r="F69">
@@ -3125,7 +3125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>8645</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>2898</v>
       </c>
       <c r="E70" s="1">
-        <f>B70/D70</f>
+        <f t="shared" si="2"/>
         <v>2.3281573498964803</v>
       </c>
       <c r="F70">
@@ -3164,7 +3164,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>8675</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>2860</v>
       </c>
       <c r="E71" s="1">
-        <f>B71/D71</f>
+        <f t="shared" si="2"/>
         <v>2.3566433566433567</v>
       </c>
       <c r="F71">
@@ -3203,7 +3203,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>8706</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>2882</v>
       </c>
       <c r="E72" s="1">
-        <f>B72/D72</f>
+        <f t="shared" si="2"/>
         <v>2.3601665510062455</v>
       </c>
       <c r="F72">
@@ -3242,7 +3242,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>8736</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>2791</v>
       </c>
       <c r="E73" s="1">
-        <f>B73/D73</f>
+        <f t="shared" si="2"/>
         <v>2.4177714080974559</v>
       </c>
       <c r="F73">
@@ -3281,7 +3281,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>8767</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>2712</v>
       </c>
       <c r="E74" s="1">
-        <f>B74/D74</f>
+        <f t="shared" si="2"/>
         <v>2.4756637168141591</v>
       </c>
       <c r="F74">
@@ -3320,7 +3320,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>8798</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>2737</v>
       </c>
       <c r="E75" s="1">
-        <f>B75/D75</f>
+        <f t="shared" si="2"/>
         <v>2.474607234198027</v>
       </c>
       <c r="F75">
@@ -3359,7 +3359,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>8827</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>2710</v>
       </c>
       <c r="E76" s="1">
-        <f>B76/D76</f>
+        <f t="shared" si="2"/>
         <v>2.5044280442804427</v>
       </c>
       <c r="F76">
@@ -3398,7 +3398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>8858</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>2678</v>
       </c>
       <c r="E77" s="1">
-        <f>B77/D77</f>
+        <f t="shared" si="2"/>
         <v>2.5399551904406272</v>
       </c>
       <c r="F77">
@@ -3437,7 +3437,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>8888</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>2659</v>
       </c>
       <c r="E78" s="1">
-        <f>B78/D78</f>
+        <f t="shared" si="2"/>
         <v>2.5675065814215872</v>
       </c>
       <c r="F78">
@@ -3476,7 +3476,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>8919</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>2650</v>
       </c>
       <c r="E79" s="1">
-        <f>B79/D79</f>
+        <f t="shared" si="2"/>
         <v>2.5852830188679246</v>
       </c>
       <c r="F79">
@@ -3515,7 +3515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>8949</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>2689</v>
       </c>
       <c r="E80" s="1">
-        <f>B80/D80</f>
+        <f t="shared" si="2"/>
         <v>2.5708441799925623</v>
       </c>
       <c r="F80">
@@ -3554,7 +3554,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>8980</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>2686</v>
       </c>
       <c r="E81" s="1">
-        <f>B81/D81</f>
+        <f t="shared" si="2"/>
         <v>2.5763216679076693</v>
       </c>
       <c r="F81">
@@ -3593,7 +3593,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>9011</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>2662</v>
       </c>
       <c r="E82" s="1">
-        <f>B82/D82</f>
+        <f t="shared" si="2"/>
         <v>2.5867768595041323</v>
       </c>
       <c r="F82">
@@ -3632,7 +3632,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>9041</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>2768</v>
       </c>
       <c r="E83" s="1">
-        <f>B83/D83</f>
+        <f t="shared" si="2"/>
         <v>2.5252890173410405</v>
       </c>
       <c r="F83">
@@ -3671,7 +3671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>9072</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>2768</v>
       </c>
       <c r="E84" s="1">
-        <f>B84/D84</f>
+        <f t="shared" si="2"/>
         <v>2.5317919075144508</v>
       </c>
       <c r="F84">
@@ -3710,7 +3710,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>9102</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>2807</v>
       </c>
       <c r="E85" s="1">
-        <f>B85/D85</f>
+        <f t="shared" si="2"/>
         <v>2.5005343783398648</v>
       </c>
       <c r="F85">
@@ -3749,7 +3749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>9133</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>2871</v>
       </c>
       <c r="E86" s="1">
-        <f>B86/D86</f>
+        <f t="shared" si="2"/>
         <v>2.4406130268199235</v>
       </c>
       <c r="F86">
@@ -3788,7 +3788,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>9164</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>3000</v>
       </c>
       <c r="E87" s="1">
-        <f>B87/D87</f>
+        <f t="shared" si="2"/>
         <v>2.359</v>
       </c>
       <c r="F87">
@@ -3827,7 +3827,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>9192</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>2922</v>
       </c>
       <c r="E88" s="1">
-        <f>B88/D88</f>
+        <f t="shared" si="2"/>
         <v>2.3867214236824092</v>
       </c>
       <c r="F88">
@@ -3866,7 +3866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>9223</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>2925</v>
       </c>
       <c r="E89" s="1">
-        <f>B89/D89</f>
+        <f t="shared" si="2"/>
         <v>2.3863247863247863</v>
       </c>
       <c r="F89">
@@ -3905,7 +3905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>9253</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>2918</v>
       </c>
       <c r="E90" s="1">
-        <f>B90/D90</f>
+        <f t="shared" si="2"/>
         <v>2.3947909527073339</v>
       </c>
       <c r="F90">
@@ -3944,7 +3944,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>9284</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>2878</v>
       </c>
       <c r="E91" s="1">
-        <f>B91/D91</f>
+        <f t="shared" si="2"/>
         <v>2.4152189020152885</v>
       </c>
       <c r="F91">
@@ -3983,7 +3983,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>9314</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>2937</v>
       </c>
       <c r="E92" s="1">
-        <f>B92/D92</f>
+        <f t="shared" si="2"/>
         <v>2.3891726251276815</v>
       </c>
       <c r="F92">
@@ -4022,7 +4022,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>9345</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>2923</v>
       </c>
       <c r="E93" s="1">
-        <f>B93/D93</f>
+        <f t="shared" si="2"/>
         <v>2.4009579199452618</v>
       </c>
       <c r="F93">
@@ -4061,7 +4061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>9376</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>2941</v>
       </c>
       <c r="E94" s="1">
-        <f>B94/D94</f>
+        <f t="shared" si="2"/>
         <v>2.3923835430125808</v>
       </c>
       <c r="F94">
@@ -4100,7 +4100,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>9406</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2934</v>
       </c>
       <c r="E95" s="1">
-        <f>B95/D95</f>
+        <f t="shared" si="2"/>
         <v>2.4042263122017724</v>
       </c>
       <c r="F95">
@@ -4139,7 +4139,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>9437</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>2944</v>
       </c>
       <c r="E96" s="1">
-        <f>B96/D96</f>
+        <f t="shared" si="2"/>
         <v>2.3960597826086958</v>
       </c>
       <c r="F96">
@@ -4178,7 +4178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>9467</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>3049</v>
       </c>
       <c r="E97" s="1">
-        <f>B97/D97</f>
+        <f t="shared" si="2"/>
         <v>2.348638897999344</v>
       </c>
       <c r="F97">
@@ -4217,7 +4217,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>9498</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>2982</v>
       </c>
       <c r="E98" s="1">
-        <f>B98/D98</f>
+        <f t="shared" ref="E98:E129" si="3">B98/D98</f>
         <v>2.3832997987927564</v>
       </c>
       <c r="F98">
@@ -4256,7 +4256,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>9529</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>2995</v>
       </c>
       <c r="E99" s="1">
-        <f>B99/D99</f>
+        <f t="shared" si="3"/>
         <v>2.3809682804674459</v>
       </c>
       <c r="F99">
@@ -4295,7 +4295,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>9557</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>2969</v>
       </c>
       <c r="E100" s="1">
-        <f>B100/D100</f>
+        <f t="shared" si="3"/>
         <v>2.3994610980127988</v>
       </c>
       <c r="F100">
@@ -4334,7 +4334,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>9588</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>3015</v>
       </c>
       <c r="E101" s="1">
-        <f>B101/D101</f>
+        <f t="shared" si="3"/>
         <v>2.3767827529021557</v>
       </c>
       <c r="F101">
@@ -4373,7 +4373,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>9618</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>2980</v>
       </c>
       <c r="E102" s="1">
-        <f>B102/D102</f>
+        <f t="shared" si="3"/>
         <v>2.3912751677852349</v>
       </c>
       <c r="F102">
@@ -4412,7 +4412,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>9649</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>2970</v>
       </c>
       <c r="E103" s="1">
-        <f>B103/D103</f>
+        <f t="shared" si="3"/>
         <v>2.4006734006734005</v>
       </c>
       <c r="F103">
@@ -4451,7 +4451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>9679</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>2989</v>
       </c>
       <c r="E104" s="1">
-        <f>B104/D104</f>
+        <f t="shared" si="3"/>
         <v>2.3997992639678825</v>
       </c>
       <c r="F104">
@@ -4490,7 +4490,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>9710</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>2944</v>
       </c>
       <c r="E105" s="1">
-        <f>B105/D105</f>
+        <f t="shared" si="3"/>
         <v>2.421875</v>
       </c>
       <c r="F105">
@@ -4529,7 +4529,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>9741</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>2969</v>
       </c>
       <c r="E106" s="1">
-        <f>B106/D106</f>
+        <f t="shared" si="3"/>
         <v>2.407544627820815</v>
       </c>
       <c r="F106">
@@ -4568,7 +4568,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>9771</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>2907</v>
       </c>
       <c r="E107" s="1">
-        <f>B107/D107</f>
+        <f t="shared" si="3"/>
         <v>2.4399724802201583</v>
       </c>
       <c r="F107">
@@ -4607,7 +4607,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>9802</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>2866</v>
       </c>
       <c r="E108" s="1">
-        <f>B108/D108</f>
+        <f t="shared" si="3"/>
         <v>2.4619678995115142</v>
       </c>
       <c r="F108">
@@ -4646,7 +4646,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>9832</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>2888</v>
       </c>
       <c r="E109" s="1">
-        <f>B109/D109</f>
+        <f t="shared" si="3"/>
         <v>2.4560249307479225</v>
       </c>
       <c r="F109">
@@ -4685,7 +4685,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>9863</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>2815</v>
       </c>
       <c r="E110" s="1">
-        <f>B110/D110</f>
+        <f t="shared" si="3"/>
         <v>2.5193605683836591</v>
       </c>
       <c r="F110">
@@ -4724,7 +4724,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>9894</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>2785</v>
       </c>
       <c r="E111" s="1">
-        <f>B111/D111</f>
+        <f t="shared" si="3"/>
         <v>2.5436265709156194</v>
       </c>
       <c r="F111">
@@ -4763,7 +4763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>9922</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>2900</v>
       </c>
       <c r="E112" s="1">
-        <f>B112/D112</f>
+        <f t="shared" si="3"/>
         <v>2.4862068965517241</v>
       </c>
       <c r="F112">
@@ -4802,7 +4802,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>9953</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>2888</v>
       </c>
       <c r="E113" s="1">
-        <f>B113/D113</f>
+        <f t="shared" si="3"/>
         <v>2.4968836565096955</v>
       </c>
       <c r="F113">
@@ -4841,7 +4841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>9983</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>2875</v>
       </c>
       <c r="E114" s="1">
-        <f>B114/D114</f>
+        <f t="shared" si="3"/>
         <v>2.5029565217391303</v>
       </c>
       <c r="F114">
@@ -4880,7 +4880,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>10014</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>2938</v>
       </c>
       <c r="E115" s="1">
-        <f>B115/D115</f>
+        <f t="shared" si="3"/>
         <v>2.4635806671204903</v>
       </c>
       <c r="F115">
@@ -4919,7 +4919,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>10044</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>2905</v>
       </c>
       <c r="E116" s="1">
-        <f>B116/D116</f>
+        <f t="shared" si="3"/>
         <v>2.4777969018932873</v>
       </c>
       <c r="F116">
@@ -4958,7 +4958,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>10075</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>2860</v>
       </c>
       <c r="E117" s="1">
-        <f>B117/D117</f>
+        <f t="shared" si="3"/>
         <v>2.5038461538461538</v>
       </c>
       <c r="F117">
@@ -4997,7 +4997,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>10106</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>2916</v>
       </c>
       <c r="E118" s="1">
-        <f>B118/D118</f>
+        <f t="shared" si="3"/>
         <v>2.4691358024691357</v>
       </c>
       <c r="F118">
@@ -5036,7 +5036,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>10136</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>2892</v>
       </c>
       <c r="E119" s="1">
-        <f>B119/D119</f>
+        <f t="shared" si="3"/>
         <v>2.4709543568464731</v>
       </c>
       <c r="F119">
@@ -5075,7 +5075,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>10167</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>2982</v>
       </c>
       <c r="E120" s="1">
-        <f>B120/D120</f>
+        <f t="shared" si="3"/>
         <v>2.3963782696177063</v>
       </c>
       <c r="F120">
@@ -5114,7 +5114,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>10197</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>3091</v>
       </c>
       <c r="E121" s="1">
-        <f>B121/D121</f>
+        <f t="shared" si="3"/>
         <v>2.3238434163701069</v>
       </c>
       <c r="F121">
@@ -5153,7 +5153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>10228</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>3023</v>
       </c>
       <c r="E122" s="1">
-        <f>B122/D122</f>
+        <f t="shared" si="3"/>
         <v>2.3516374462454515</v>
       </c>
       <c r="F122">
@@ -5192,7 +5192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>10259</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>3039</v>
       </c>
       <c r="E123" s="1">
-        <f>B123/D123</f>
+        <f t="shared" si="3"/>
         <v>2.3409016123724911</v>
       </c>
       <c r="F123">
@@ -5231,7 +5231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>10288</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>3146</v>
       </c>
       <c r="E124" s="1">
-        <f>B124/D124</f>
+        <f t="shared" si="3"/>
         <v>2.2771773680864591</v>
       </c>
       <c r="F124">
@@ -5270,7 +5270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>10319</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>3232</v>
       </c>
       <c r="E125" s="1">
-        <f>B125/D125</f>
+        <f t="shared" si="3"/>
         <v>2.2311262376237622</v>
       </c>
       <c r="F125">
@@ -5309,7 +5309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>10349</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>3286</v>
       </c>
       <c r="E126" s="1">
-        <f>B126/D126</f>
+        <f t="shared" si="3"/>
         <v>2.1786366402921487</v>
       </c>
       <c r="F126">
@@ -5348,7 +5348,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>10380</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>3328</v>
       </c>
       <c r="E127" s="1">
-        <f>B127/D127</f>
+        <f t="shared" si="3"/>
         <v>2.1484375</v>
       </c>
       <c r="F127">
@@ -5387,7 +5387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>10410</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>3245</v>
       </c>
       <c r="E128" s="1">
-        <f>B128/D128</f>
+        <f t="shared" si="3"/>
         <v>2.1790446841294298</v>
       </c>
       <c r="F128">
@@ -5426,7 +5426,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>10441</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>3255</v>
       </c>
       <c r="E129" s="1">
-        <f>B129/D129</f>
+        <f t="shared" si="3"/>
         <v>2.1784946236559142</v>
       </c>
       <c r="F129">
@@ -5465,7 +5465,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>10472</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>3228</v>
       </c>
       <c r="E130" s="1">
-        <f>B130/D130</f>
+        <f t="shared" ref="E130:E161" si="4">B130/D130</f>
         <v>2.1889714993804215</v>
       </c>
       <c r="F130">
@@ -5504,7 +5504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>10502</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>3187</v>
       </c>
       <c r="E131" s="1">
-        <f>B131/D131</f>
+        <f t="shared" si="4"/>
         <v>2.2096015061186067</v>
       </c>
       <c r="F131">
@@ -5543,7 +5543,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>10533</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>3344</v>
       </c>
       <c r="E132" s="1">
-        <f>B132/D132</f>
+        <f t="shared" si="4"/>
         <v>2.1486244019138754</v>
       </c>
       <c r="F132">
@@ -5582,7 +5582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>10563</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>3264</v>
       </c>
       <c r="E133" s="1">
-        <f>B133/D133</f>
+        <f t="shared" si="4"/>
         <v>2.1807598039215685</v>
       </c>
       <c r="F133">
@@ -5621,7 +5621,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>10594</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>3315</v>
       </c>
       <c r="E134" s="1">
-        <f>B134/D134</f>
+        <f t="shared" si="4"/>
         <v>2.1583710407239818</v>
       </c>
       <c r="F134">
@@ -5660,7 +5660,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>10625</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>3273</v>
       </c>
       <c r="E135" s="1">
-        <f>B135/D135</f>
+        <f t="shared" si="4"/>
         <v>2.1811793461655973</v>
       </c>
       <c r="F135">
@@ -5699,7 +5699,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>10653</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>3251</v>
       </c>
       <c r="E136" s="1">
-        <f>B136/D136</f>
+        <f t="shared" si="4"/>
         <v>2.1999384804675484</v>
       </c>
       <c r="F136">
@@ -5738,7 +5738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>10684</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>3046</v>
       </c>
       <c r="E137" s="1">
-        <f>B137/D137</f>
+        <f t="shared" si="4"/>
         <v>2.3043335521996062</v>
       </c>
       <c r="F137">
@@ -5777,7 +5777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>10714</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>3034</v>
       </c>
       <c r="E138" s="1">
-        <f>B138/D138</f>
+        <f t="shared" si="4"/>
         <v>2.3230059327620305</v>
       </c>
       <c r="F138">
@@ -5816,7 +5816,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>10745</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>3065</v>
       </c>
       <c r="E139" s="1">
-        <f>B139/D139</f>
+        <f t="shared" si="4"/>
         <v>2.3171288743882545</v>
       </c>
       <c r="F139">
@@ -5855,7 +5855,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>10775</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>3069</v>
       </c>
       <c r="E140" s="1">
-        <f>B140/D140</f>
+        <f t="shared" si="4"/>
         <v>2.3209514499837081</v>
       </c>
       <c r="F140">
@@ -5894,7 +5894,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>10806</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3082</v>
       </c>
       <c r="E141" s="1">
-        <f>B141/D141</f>
+        <f t="shared" si="4"/>
         <v>2.3215444516547694</v>
       </c>
       <c r="F141">
@@ -5933,7 +5933,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>10837</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>2990</v>
       </c>
       <c r="E142" s="1">
-        <f>B142/D142</f>
+        <f t="shared" si="4"/>
         <v>2.3662207357859533</v>
       </c>
       <c r="F142">
@@ -5972,7 +5972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>10867</v>
       </c>
@@ -5986,7 +5986,7 @@
         <v>3246</v>
       </c>
       <c r="E143" s="1">
-        <f>B143/D143</f>
+        <f t="shared" si="4"/>
         <v>2.2627849661121382</v>
       </c>
       <c r="F143">
@@ -6011,7 +6011,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>10898</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>3072</v>
       </c>
       <c r="E144" s="1">
-        <f>B144/D144</f>
+        <f t="shared" si="4"/>
         <v>2.328125</v>
       </c>
       <c r="F144">
@@ -6050,7 +6050,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>10928</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>2981</v>
       </c>
       <c r="E145" s="1">
-        <f>B145/D145</f>
+        <f t="shared" si="4"/>
         <v>2.3408252264340823</v>
       </c>
       <c r="F145">
@@ -6089,7 +6089,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>10959</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>2976</v>
       </c>
       <c r="E146" s="1">
-        <f>B146/D146</f>
+        <f t="shared" si="4"/>
         <v>2.3454301075268815</v>
       </c>
       <c r="F146">
@@ -6128,7 +6128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>10990</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>2933</v>
       </c>
       <c r="E147" s="1">
-        <f>B147/D147</f>
+        <f t="shared" si="4"/>
         <v>2.3862938970337537</v>
       </c>
       <c r="F147">
@@ -6167,7 +6167,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>11018</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>2827</v>
       </c>
       <c r="E148" s="1">
-        <f>B148/D148</f>
+        <f t="shared" si="4"/>
         <v>2.463035019455253</v>
       </c>
       <c r="F148">
@@ -6206,7 +6206,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>11049</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>2704</v>
       </c>
       <c r="E149" s="1">
-        <f>B149/D149</f>
+        <f t="shared" si="4"/>
         <v>2.554733727810651</v>
       </c>
       <c r="F149">
@@ -6245,7 +6245,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>11079</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>2675</v>
       </c>
       <c r="E150" s="1">
-        <f>B150/D150</f>
+        <f t="shared" si="4"/>
         <v>2.5813084112149531</v>
       </c>
       <c r="F150">
@@ -6284,7 +6284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>11110</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>2660</v>
       </c>
       <c r="E151" s="1">
-        <f>B151/D151</f>
+        <f t="shared" si="4"/>
         <v>2.5969924812030074</v>
       </c>
       <c r="F151">
@@ -6323,7 +6323,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>11140</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>2695</v>
       </c>
       <c r="E152" s="1">
-        <f>B152/D152</f>
+        <f t="shared" si="4"/>
         <v>2.5695732838589982</v>
       </c>
       <c r="F152">
@@ -6362,7 +6362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>11171</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>2739</v>
       </c>
       <c r="E153" s="1">
-        <f>B153/D153</f>
+        <f t="shared" si="4"/>
         <v>2.5385177071924061</v>
       </c>
       <c r="F153">
@@ -6401,7 +6401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>11202</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>2605</v>
       </c>
       <c r="E154" s="1">
-        <f>B154/D154</f>
+        <f t="shared" si="4"/>
         <v>2.6214971209213052</v>
       </c>
       <c r="F154">
@@ -6440,7 +6440,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>11232</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>2569</v>
       </c>
       <c r="E155" s="1">
-        <f>B155/D155</f>
+        <f t="shared" si="4"/>
         <v>2.6535616971584273</v>
       </c>
       <c r="F155">
@@ -6479,7 +6479,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>11263</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>2651</v>
       </c>
       <c r="E156" s="1">
-        <f>B156/D156</f>
+        <f t="shared" si="4"/>
         <v>2.6159939645416825</v>
       </c>
       <c r="F156">
@@ -6518,7 +6518,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>11293</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>2819</v>
       </c>
       <c r="E157" s="1">
-        <f>B157/D157</f>
+        <f t="shared" si="4"/>
         <v>2.5274920184462575</v>
       </c>
       <c r="F157">
@@ -6557,7 +6557,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>11324</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>2796</v>
       </c>
       <c r="E158" s="1">
-        <f>B158/D158</f>
+        <f t="shared" si="4"/>
         <v>2.5579399141630903</v>
       </c>
       <c r="F158">
@@ -6593,7 +6593,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>11355</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>2698</v>
       </c>
       <c r="E159" s="1">
-        <f>B159/D159</f>
+        <f t="shared" si="4"/>
         <v>2.6226834692364713</v>
       </c>
       <c r="F159">
@@ -6629,7 +6629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>11383</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>2680</v>
       </c>
       <c r="E160" s="1">
-        <f>B160/D160</f>
+        <f t="shared" si="4"/>
         <v>2.6455223880597014</v>
       </c>
       <c r="F160">
@@ -6665,7 +6665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>11414</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>2680</v>
       </c>
       <c r="E161" s="1">
-        <f>B161/D161</f>
+        <f t="shared" si="4"/>
         <v>2.6563432835820895</v>
       </c>
       <c r="F161">
@@ -6701,7 +6701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>11444</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>2619</v>
       </c>
       <c r="E162" s="1">
-        <f>B162/D162</f>
+        <f t="shared" ref="E162:E193" si="5">B162/D162</f>
         <v>2.7224131347842686</v>
       </c>
       <c r="F162">
@@ -6737,7 +6737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>11475</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>2633</v>
       </c>
       <c r="E163" s="1">
-        <f>B163/D163</f>
+        <f t="shared" si="5"/>
         <v>2.7732624382833269</v>
       </c>
       <c r="F163">
@@ -6773,7 +6773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>11505</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>2659</v>
       </c>
       <c r="E164" s="1">
-        <f>B164/D164</f>
+        <f t="shared" si="5"/>
         <v>2.7532907107935314</v>
       </c>
       <c r="F164">
@@ -6809,7 +6809,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>11536</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>2667</v>
       </c>
       <c r="E165" s="1">
-        <f>B165/D165</f>
+        <f t="shared" si="5"/>
         <v>2.7652793400824898</v>
       </c>
       <c r="F165">
@@ -6845,7 +6845,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>11567</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>3044</v>
       </c>
       <c r="E166" s="1">
-        <f>B166/D166</f>
+        <f t="shared" si="5"/>
         <v>2.4632063074901445</v>
       </c>
       <c r="F166">
@@ -6881,7 +6881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>11597</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>3565</v>
       </c>
       <c r="E167" s="1">
-        <f>B167/D167</f>
+        <f t="shared" si="5"/>
         <v>2.1234221598877983</v>
       </c>
       <c r="F167">
@@ -6917,7 +6917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>11628</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>3331</v>
       </c>
       <c r="E168" s="1">
-        <f>B168/D168</f>
+        <f t="shared" si="5"/>
         <v>2.2389672770939657</v>
       </c>
       <c r="F168">
@@ -6953,7 +6953,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>11658</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>3562</v>
       </c>
       <c r="E169" s="1">
-        <f>B169/D169</f>
+        <f t="shared" si="5"/>
         <v>2.1715328467153285</v>
       </c>
       <c r="F169">
@@ -6989,7 +6989,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>11689</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>3575</v>
       </c>
       <c r="E170" s="1">
-        <f>B170/D170</f>
+        <f t="shared" si="5"/>
         <v>2.1549650349650351</v>
       </c>
       <c r="F170">
@@ -7025,7 +7025,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>11720</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>3470</v>
       </c>
       <c r="E171" s="1">
-        <f>B171/D171</f>
+        <f t="shared" si="5"/>
         <v>2.1720461095100863</v>
       </c>
       <c r="F171">
@@ -7061,7 +7061,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>11749</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>3436</v>
       </c>
       <c r="E172" s="1">
-        <f>B172/D172</f>
+        <f t="shared" si="5"/>
         <v>2.1941210710128054</v>
       </c>
       <c r="F172">
@@ -7097,7 +7097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>11780</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>3564</v>
       </c>
       <c r="E173" s="1">
-        <f>B173/D173</f>
+        <f t="shared" si="5"/>
         <v>2.1447811447811449</v>
       </c>
       <c r="F173">
@@ -7133,7 +7133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>11810</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>3845</v>
       </c>
       <c r="E174" s="1">
-        <f>B174/D174</f>
+        <f t="shared" si="5"/>
         <v>2.0052015604681404</v>
       </c>
       <c r="F174">
@@ -7169,7 +7169,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>11841</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>4156</v>
       </c>
       <c r="E175" s="1">
-        <f>B175/D175</f>
+        <f t="shared" si="5"/>
         <v>1.873917228103946</v>
       </c>
       <c r="F175">
@@ -7205,7 +7205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>11871</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>4171</v>
       </c>
       <c r="E176" s="1">
-        <f>B176/D176</f>
+        <f t="shared" si="5"/>
         <v>1.8839606808918725</v>
       </c>
       <c r="F176">
@@ -7241,7 +7241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>11902</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>4049</v>
       </c>
       <c r="E177" s="1">
-        <f>B177/D177</f>
+        <f t="shared" si="5"/>
         <v>1.9387503087182021</v>
       </c>
       <c r="F177">
@@ -7277,7 +7277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>11933</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>3991</v>
       </c>
       <c r="E178" s="1">
-        <f>B178/D178</f>
+        <f t="shared" si="5"/>
         <v>1.9787020796792785</v>
       </c>
       <c r="F178">
@@ -7313,7 +7313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>11963</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>3919</v>
       </c>
       <c r="E179" s="1">
-        <f>B179/D179</f>
+        <f t="shared" si="5"/>
         <v>2.0147996937994388</v>
       </c>
       <c r="F179">
@@ -7349,7 +7349,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>11994</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>3925</v>
       </c>
       <c r="E180" s="1">
-        <f>B180/D180</f>
+        <f t="shared" si="5"/>
         <v>2.032611464968153</v>
       </c>
       <c r="F180">
@@ -7385,7 +7385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>12024</v>
       </c>
@@ -7400,7 +7400,7 @@
         <v>3802</v>
       </c>
       <c r="E181" s="1">
-        <f>B181/D181</f>
+        <f t="shared" si="5"/>
         <v>2.1115202524986847</v>
       </c>
       <c r="F181">
@@ -7422,7 +7422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>12055</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>12086</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>12114</v>
       </c>
@@ -7482,7 +7482,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>12145</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>12175</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>12206</v>
       </c>
@@ -7542,7 +7542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>12236</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>12267</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>12298</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>12328</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>12359</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>12389</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>12420</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>12451</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>12479</v>
       </c>
@@ -7713,7 +7713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>12510</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>12540</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>12571</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>12601</v>
       </c>
@@ -7781,7 +7781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>12632</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>12663</v>
       </c>
@@ -7815,7 +7815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>12693</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>12724</v>
       </c>
@@ -7849,7 +7849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>12754</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>12785</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>12816</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>12844</v>
       </c>
@@ -7917,7 +7917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>12875</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>12905</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>12936</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>12966</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>12997</v>
       </c>
@@ -8002,7 +8002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>13028</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>13058</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>13089</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>13119</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>13150</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>13181</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>13210</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>13241</v>
       </c>
@@ -8138,7 +8138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>13271</v>
       </c>
@@ -8155,7 +8155,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>13302</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>13332</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>13363</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>13394</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>13424</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>13455</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>13485</v>
       </c>
@@ -8274,454 +8274,454 @@
         <v>54</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="2"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="2"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" s="2"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="2"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="2"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A305" s="2"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A306" s="2"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A307" s="2"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="2"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A309" s="2"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A310" s="2"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A311" s="2"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A312" s="2"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="2"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A314" s="2"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A315" s="2"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="2"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" s="2"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="2"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" s="2"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A320" s="2"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A321" s="2"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" s="2"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A323" s="2"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A324" s="2"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="2"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A326" s="2"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A327" s="2"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A328" s="2"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A329" s="2"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A330" s="2"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A331" s="2"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A332" s="2"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="2"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A334" s="2"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A335" s="2"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A336" s="2"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A337" s="2"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A338" s="2"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="2"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A340" s="2"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A341" s="2"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A342" s="2"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A343" s="2"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A344" s="2"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A345" s="2"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="2"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A347" s="2"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A348" s="2"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="2"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" s="2"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A351" s="2"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A352" s="2"/>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A353" s="2"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A354" s="2"/>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="2"/>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A356" s="2"/>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A357" s="2"/>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="2"/>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A359" s="2"/>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="2"/>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A361" s="2"/>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A362" s="2"/>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="2"/>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A364" s="2"/>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A365" s="2"/>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A366" s="2"/>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A367" s="2"/>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="2"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="2"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="2"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="2"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="2"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="2"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="2"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="2"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="2"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="2"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="2"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="2"/>
     </row>
   </sheetData>

</xml_diff>